<commit_message>
Updated startup.c and pin spreadsheet
</commit_message>
<xml_diff>
--- a/docs/DogBoneSDRAMv1.xlsx
+++ b/docs/DogBoneSDRAMv1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12345"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="212">
   <si>
     <t>B0_01</t>
   </si>
@@ -711,6 +711,27 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>3:7</t>
+  </si>
+  <si>
+    <t>1.22</t>
+  </si>
+  <si>
+    <t>Serial2(3) TX</t>
+  </si>
+  <si>
+    <t>Wire2(3) SDA</t>
+  </si>
+  <si>
+    <t>3:6</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA2</t>
   </si>
 </sst>
 </file>
@@ -1133,14 +1154,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1359,6 +1372,13 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
@@ -1403,7 +1423,8 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <bgColor auto="1"/>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1451,7 +1472,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>590549</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -1490,7 +1511,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O45" totalsRowShown="0" headerRowDxfId="16" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:O45" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:O45"/>
   <sortState ref="A2:N45">
     <sortCondition ref="B1:B45"/>
@@ -1498,18 +1519,18 @@
   <tableColumns count="15">
     <tableColumn id="1" name="Pin" dataDxfId="14"/>
     <tableColumn id="2" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" name="GPIO" dataDxfId="15"/>
-    <tableColumn id="4" name="Serial" dataDxfId="12"/>
-    <tableColumn id="5" name="I2C" dataDxfId="11"/>
-    <tableColumn id="6" name="SPI" dataDxfId="10"/>
-    <tableColumn id="7" name="PWM" dataDxfId="9"/>
-    <tableColumn id="8" name="CAN" dataDxfId="8"/>
-    <tableColumn id="9" name="Audio" dataDxfId="7"/>
-    <tableColumn id="10" name="XBAR" dataDxfId="6"/>
-    <tableColumn id="11" name="FlexIO" dataDxfId="5"/>
-    <tableColumn id="12" name="Analog" dataDxfId="4"/>
-    <tableColumn id="13" name="SD/CSI/LCD" dataDxfId="3"/>
-    <tableColumn id="14" name="Column1" dataDxfId="2"/>
+    <tableColumn id="3" name="GPIO" dataDxfId="12"/>
+    <tableColumn id="4" name="Serial" dataDxfId="11"/>
+    <tableColumn id="5" name="I2C" dataDxfId="10"/>
+    <tableColumn id="6" name="SPI" dataDxfId="9"/>
+    <tableColumn id="7" name="PWM" dataDxfId="8"/>
+    <tableColumn id="8" name="CAN" dataDxfId="7"/>
+    <tableColumn id="9" name="Audio" dataDxfId="6"/>
+    <tableColumn id="10" name="XBAR" dataDxfId="5"/>
+    <tableColumn id="11" name="FlexIO" dataDxfId="4"/>
+    <tableColumn id="12" name="Analog" dataDxfId="3"/>
+    <tableColumn id="13" name="SD/CSI/LCD" dataDxfId="2"/>
+    <tableColumn id="14" name="Column1" dataDxfId="1"/>
     <tableColumn id="15" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1805,8 +1826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3510,8 +3531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI46"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3523,7 +3544,7 @@
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5014,30 +5035,38 @@
       <c r="B34" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="47">
-        <v>1.22</v>
+      <c r="C34" s="47" t="s">
+        <v>207</v>
       </c>
       <c r="D34" s="47" t="s">
-        <v>72</v>
+        <v>208</v>
       </c>
       <c r="E34" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
+        <v>209</v>
+      </c>
+      <c r="F34" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="47" t="s">
+        <v>174</v>
+      </c>
       <c r="I34" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="J34" s="47"/>
-      <c r="K34" s="55">
-        <v>0.12916666666666668</v>
+      <c r="J34" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="K34" s="55" t="s">
+        <v>210</v>
       </c>
       <c r="L34" s="47" t="s">
         <v>75</v>
       </c>
       <c r="M34" s="69" t="s">
-        <v>76</v>
+        <v>211</v>
       </c>
       <c r="V34" s="65" t="s">
         <v>172</v>
@@ -5071,8 +5100,8 @@
       <c r="B35" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="C35" s="44">
-        <v>1.23</v>
+      <c r="C35" s="44" t="s">
+        <v>205</v>
       </c>
       <c r="D35" s="44" t="s">
         <v>159</v>
@@ -5080,15 +5109,23 @@
       <c r="E35" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
+      <c r="F35" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="H35" s="44" t="s">
+        <v>174</v>
+      </c>
       <c r="I35" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="J35" s="44"/>
-      <c r="K35" s="53">
-        <v>0.12986111111111112</v>
+      <c r="J35" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="K35" s="53" t="s">
+        <v>206</v>
       </c>
       <c r="L35" s="44" t="s">
         <v>162</v>
@@ -5478,7 +5515,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
DB5 - preliminary page
</commit_message>
<xml_diff>
--- a/docs/DogBoneSDRAMv1.xlsx
+++ b/docs/DogBoneSDRAMv1.xlsx
@@ -1,29 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\EVKB_1060\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50528214-1300-4CD8-B4CA-46641D7B50B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C05FE3-A1A7-4A62-8D80-956C411AF3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="540" windowWidth="29535" windowHeight="18630" tabRatio="400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="2400" windowWidth="33465" windowHeight="14415" tabRatio="400" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Mux" sheetId="4" r:id="rId4"/>
+    <sheet name="DB5 Card like" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="1047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="1064">
   <si>
     <t>B0_01</t>
   </si>
@@ -3301,6 +3315,133 @@
   </si>
   <si>
     <t>New T5 15/A1</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>51</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 37 on t41</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>36 on t41</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 35 on t41</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>61</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 34 ont41</t>
+    </r>
+  </si>
+  <si>
+    <t>AD_B1_04</t>
+  </si>
+  <si>
+    <t>AD_B1_05</t>
+  </si>
+  <si>
+    <t>AD_B1_12</t>
+  </si>
+  <si>
+    <t>AD_B1_13</t>
+  </si>
+  <si>
+    <t>Serial3(2) RX</t>
+  </si>
+  <si>
+    <t>15/A1</t>
+  </si>
+  <si>
+    <t>A1:8, A2:8</t>
+  </si>
+  <si>
+    <t>1.21</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>A1:9</t>
+  </si>
+  <si>
+    <t>A1:10</t>
   </si>
 </sst>
 </file>
@@ -3449,7 +3590,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3536,12 +3677,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3559,7 +3694,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -3834,13 +3969,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4088,9 +4234,10 @@
     <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4100,8 +4247,27 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4549,6 +4715,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>795618</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>634234</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D640AD66-4DED-F7F8-1DDA-22EBF67E00B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9749118" y="123266"/>
+          <a:ext cx="4892469" cy="8516470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:O45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:O45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
@@ -6528,7 +6760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI46"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
@@ -9111,21 +9343,21 @@
       <c r="M10" s="96"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="129" t="s">
         <v>263</v>
       </c>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
-      <c r="J11" s="129"/>
-      <c r="K11" s="129"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="130"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="130"/>
+      <c r="L11" s="130"/>
+      <c r="M11" s="131"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="86" t="s">
@@ -9261,8 +9493,8 @@
   </sheetPr>
   <dimension ref="A2:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9670,7 +9902,7 @@
       <c r="F15" s="108" t="s">
         <v>583</v>
       </c>
-      <c r="G15" s="125" t="s">
+      <c r="G15" s="124" t="s">
         <v>392</v>
       </c>
       <c r="H15" s="111" t="s">
@@ -9693,13 +9925,13 @@
       <c r="D16" s="108" t="s">
         <v>818</v>
       </c>
-      <c r="E16" s="124" t="s">
+      <c r="E16" s="109" t="s">
         <v>463</v>
       </c>
       <c r="F16" s="108" t="s">
         <v>405</v>
       </c>
-      <c r="G16" s="125" t="s">
+      <c r="G16" s="124" t="s">
         <v>383</v>
       </c>
       <c r="H16" s="111" t="s">
@@ -9722,7 +9954,7 @@
       <c r="D17" s="108" t="s">
         <v>821</v>
       </c>
-      <c r="E17" s="124" t="s">
+      <c r="E17" s="109" t="s">
         <v>455</v>
       </c>
       <c r="F17" s="108" t="s">
@@ -9751,7 +9983,7 @@
       <c r="D18" s="108" t="s">
         <v>824</v>
       </c>
-      <c r="E18" s="124" t="s">
+      <c r="E18" s="109" t="s">
         <v>826</v>
       </c>
       <c r="F18" s="108" t="s">
@@ -9780,7 +10012,7 @@
       <c r="D19" s="108" t="s">
         <v>825</v>
       </c>
-      <c r="E19" s="124" t="s">
+      <c r="E19" s="109" t="s">
         <v>829</v>
       </c>
       <c r="F19" s="108" t="s">
@@ -9809,7 +10041,7 @@
       <c r="D20" s="110" t="s">
         <v>831</v>
       </c>
-      <c r="E20" s="124" t="s">
+      <c r="E20" s="109" t="s">
         <v>832</v>
       </c>
       <c r="F20" s="108" t="s">
@@ -9835,7 +10067,7 @@
       <c r="D21" s="110" t="s">
         <v>833</v>
       </c>
-      <c r="E21" s="124" t="s">
+      <c r="E21" s="109" t="s">
         <v>834</v>
       </c>
       <c r="F21" s="108" t="s">
@@ -9864,7 +10096,7 @@
       <c r="D22" s="110" t="s">
         <v>838</v>
       </c>
-      <c r="E22" s="124" t="s">
+      <c r="E22" s="109" t="s">
         <v>388</v>
       </c>
       <c r="F22" s="108" t="s">
@@ -9893,7 +10125,7 @@
       <c r="D23" s="110" t="s">
         <v>842</v>
       </c>
-      <c r="E23" s="124" t="s">
+      <c r="E23" s="109" t="s">
         <v>379</v>
       </c>
       <c r="F23" s="108" t="s">
@@ -10183,7 +10415,7 @@
       <c r="F33" s="112" t="s">
         <v>623</v>
       </c>
-      <c r="G33" s="132" t="s">
+      <c r="G33" s="128" t="s">
         <v>857</v>
       </c>
       <c r="H33" s="111" t="s">
@@ -10212,7 +10444,7 @@
       <c r="F34" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="G34" s="132" t="s">
+      <c r="G34" s="128" t="s">
         <v>564</v>
       </c>
       <c r="H34" s="111" t="s">
@@ -10241,7 +10473,7 @@
       <c r="F35" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="G35" s="132" t="s">
+      <c r="G35" s="128" t="s">
         <v>556</v>
       </c>
       <c r="H35" s="111" t="s">
@@ -10270,7 +10502,7 @@
       <c r="F36" s="10" t="s">
         <v>870</v>
       </c>
-      <c r="G36" s="132" t="s">
+      <c r="G36" s="128" t="s">
         <v>871</v>
       </c>
       <c r="H36" s="111" t="s">
@@ -10302,7 +10534,7 @@
       <c r="F37" s="10" t="s">
         <v>875</v>
       </c>
-      <c r="G37" s="132" t="s">
+      <c r="G37" s="128" t="s">
         <v>872</v>
       </c>
       <c r="H37" s="111" t="s">
@@ -10331,7 +10563,7 @@
       <c r="F38" s="10" t="s">
         <v>878</v>
       </c>
-      <c r="G38" s="132" t="s">
+      <c r="G38" s="128" t="s">
         <v>873</v>
       </c>
       <c r="H38" s="111" t="s">
@@ -10363,7 +10595,7 @@
       <c r="F39" s="10" t="s">
         <v>580</v>
       </c>
-      <c r="G39" s="132" t="s">
+      <c r="G39" s="128" t="s">
         <v>581</v>
       </c>
       <c r="H39" s="111" t="s">
@@ -10398,7 +10630,7 @@
       <c r="F40" s="10" t="s">
         <v>571</v>
       </c>
-      <c r="G40" s="132" t="s">
+      <c r="G40" s="128" t="s">
         <v>572</v>
       </c>
       <c r="H40" s="111" t="s">
@@ -10433,7 +10665,7 @@
       <c r="F41" s="10" t="s">
         <v>884</v>
       </c>
-      <c r="G41" s="132" t="s">
+      <c r="G41" s="128" t="s">
         <v>885</v>
       </c>
       <c r="H41" s="111" t="s">
@@ -10613,7 +10845,7 @@
       <c r="B47" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="131" t="s">
+      <c r="C47" s="127" t="s">
         <v>369</v>
       </c>
       <c r="D47" s="110" t="s">
@@ -10645,7 +10877,7 @@
       <c r="B48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="131" t="s">
+      <c r="C48" s="127" t="s">
         <v>377</v>
       </c>
       <c r="D48" s="108" t="s">
@@ -10680,7 +10912,7 @@
       <c r="B49" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="131" t="s">
+      <c r="C49" s="127" t="s">
         <v>386</v>
       </c>
       <c r="D49" s="108" t="s">
@@ -10715,7 +10947,7 @@
       <c r="B50" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C50" s="131" t="s">
+      <c r="C50" s="127" t="s">
         <v>395</v>
       </c>
       <c r="D50" s="110" t="s">
@@ -10747,7 +10979,7 @@
       <c r="B51" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C51" s="131" t="s">
+      <c r="C51" s="127" t="s">
         <v>314</v>
       </c>
       <c r="D51" s="110" t="s">
@@ -10779,7 +11011,7 @@
       <c r="B52" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="131" t="s">
+      <c r="C52" s="127" t="s">
         <v>315</v>
       </c>
       <c r="D52" s="110" t="s">
@@ -10811,7 +11043,7 @@
       <c r="B53" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="131" t="s">
+      <c r="C53" s="127" t="s">
         <v>212</v>
       </c>
       <c r="D53" s="110" t="s">
@@ -10843,7 +11075,7 @@
       <c r="B54" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="131" t="s">
+      <c r="C54" s="127" t="s">
         <v>306</v>
       </c>
       <c r="D54" s="110" t="s">
@@ -10925,7 +11157,7 @@
       <c r="F56" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="G56" s="132" t="s">
+      <c r="G56" s="128" t="s">
         <v>223</v>
       </c>
       <c r="H56" s="111" t="s">
@@ -10963,7 +11195,7 @@
       <c r="F57" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G57" s="132" t="s">
+      <c r="G57" s="128" t="s">
         <v>76</v>
       </c>
       <c r="H57" s="111" t="s">
@@ -11077,7 +11309,7 @@
       <c r="F60" s="113" t="s">
         <v>488</v>
       </c>
-      <c r="G60" s="132" t="s">
+      <c r="G60" s="128" t="s">
         <v>489</v>
       </c>
       <c r="H60" s="111" t="s">
@@ -11115,7 +11347,7 @@
       <c r="F61" s="113" t="s">
         <v>498</v>
       </c>
-      <c r="G61" s="132" t="s">
+      <c r="G61" s="128" t="s">
         <v>499</v>
       </c>
       <c r="H61" s="111" t="s">
@@ -11153,7 +11385,7 @@
       <c r="F62" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="G62" s="132" t="s">
+      <c r="G62" s="128" t="s">
         <v>507</v>
       </c>
       <c r="H62" s="111" t="s">
@@ -11188,7 +11420,7 @@
       <c r="F63" s="113" t="s">
         <v>513</v>
       </c>
-      <c r="G63" s="132" t="s">
+      <c r="G63" s="128" t="s">
         <v>514</v>
       </c>
       <c r="H63" s="111" t="s">
@@ -11287,7 +11519,7 @@
       <c r="F66" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="G66" s="132" t="s">
+      <c r="G66" s="128" t="s">
         <v>545</v>
       </c>
       <c r="H66" s="111" t="s">
@@ -11313,7 +11545,7 @@
       <c r="B67" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="131" t="s">
+      <c r="C67" s="127" t="s">
         <v>587</v>
       </c>
       <c r="D67" s="108" t="s">
@@ -11339,7 +11571,7 @@
       </c>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="127" t="s">
+      <c r="A68" s="126" t="s">
         <v>602</v>
       </c>
       <c r="B68" s="10" t="s">
@@ -11371,7 +11603,7 @@
       </c>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="127" t="s">
+      <c r="A69" s="126" t="s">
         <v>610</v>
       </c>
       <c r="B69" s="10" t="s">
@@ -11403,7 +11635,7 @@
       </c>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="127" t="s">
+      <c r="A70" s="126" t="s">
         <v>618</v>
       </c>
       <c r="B70" s="10" t="s">
@@ -11438,7 +11670,7 @@
       </c>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="127" t="s">
+      <c r="A71" s="126" t="s">
         <v>628</v>
       </c>
       <c r="B71" s="10" t="s">
@@ -11473,7 +11705,7 @@
       </c>
     </row>
     <row r="72" spans="1:12">
-      <c r="A72" s="127" t="s">
+      <c r="A72" s="126" t="s">
         <v>636</v>
       </c>
       <c r="B72" s="10" t="s">
@@ -11505,7 +11737,7 @@
       </c>
     </row>
     <row r="73" spans="1:12">
-      <c r="A73" s="127" t="s">
+      <c r="A73" s="126" t="s">
         <v>643</v>
       </c>
       <c r="B73" s="10" t="s">
@@ -11543,7 +11775,7 @@
       <c r="B74" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="131" t="s">
+      <c r="C74" s="127" t="s">
         <v>651</v>
       </c>
       <c r="D74" s="110" t="s">
@@ -11575,7 +11807,7 @@
       <c r="B75" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="131" t="s">
+      <c r="C75" s="127" t="s">
         <v>660</v>
       </c>
       <c r="D75" s="110" t="s">
@@ -11607,7 +11839,7 @@
       <c r="B76" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="131" t="s">
+      <c r="C76" s="127" t="s">
         <v>669</v>
       </c>
       <c r="D76" s="110" t="s">
@@ -11639,7 +11871,7 @@
       <c r="B77" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C77" s="131" t="s">
+      <c r="C77" s="127" t="s">
         <v>676</v>
       </c>
       <c r="D77" s="110" t="s">
@@ -11671,7 +11903,7 @@
       <c r="B78" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C78" s="131" t="s">
+      <c r="C78" s="127" t="s">
         <v>684</v>
       </c>
       <c r="D78" s="110" t="s">
@@ -11703,7 +11935,7 @@
       <c r="B79" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C79" s="131" t="s">
+      <c r="C79" s="127" t="s">
         <v>690</v>
       </c>
       <c r="D79" s="110" t="s">
@@ -11729,13 +11961,13 @@
       </c>
     </row>
     <row r="80" spans="1:12">
-      <c r="A80" s="126" t="s">
+      <c r="A80" s="125" t="s">
         <v>913</v>
       </c>
       <c r="B80" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="131" t="s">
+      <c r="C80" s="127" t="s">
         <v>910</v>
       </c>
       <c r="D80" s="108" t="s">
@@ -11761,13 +11993,13 @@
       </c>
     </row>
     <row r="81" spans="1:12">
-      <c r="A81" s="126" t="s">
+      <c r="A81" s="125" t="s">
         <v>705</v>
       </c>
       <c r="B81" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="131" t="s">
+      <c r="C81" s="127" t="s">
         <v>911</v>
       </c>
       <c r="D81" s="108" t="s">
@@ -11796,13 +12028,13 @@
       </c>
     </row>
     <row r="82" spans="1:12">
-      <c r="A82" s="126" t="s">
+      <c r="A82" s="125" t="s">
         <v>727</v>
       </c>
       <c r="B82" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="131" t="s">
+      <c r="C82" s="127" t="s">
         <v>939</v>
       </c>
       <c r="D82" s="108" t="s">
@@ -11831,13 +12063,13 @@
       </c>
     </row>
     <row r="83" spans="1:12">
-      <c r="A83" s="126" t="s">
+      <c r="A83" s="125" t="s">
         <v>734</v>
       </c>
       <c r="B83" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="131" t="s">
+      <c r="C83" s="127" t="s">
         <v>940</v>
       </c>
       <c r="D83" s="108" t="s">
@@ -11866,19 +12098,19 @@
       </c>
     </row>
     <row r="84" spans="1:12">
-      <c r="A84" s="126" t="s">
+      <c r="A84" s="125" t="s">
         <v>697</v>
       </c>
       <c r="B84" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C84" s="131" t="s">
+      <c r="C84" s="127" t="s">
         <v>941</v>
       </c>
       <c r="D84" s="108" t="s">
         <v>406</v>
       </c>
-      <c r="E84" s="132" t="s">
+      <c r="E84" s="128" t="s">
         <v>982</v>
       </c>
       <c r="F84" s="113" t="s">
@@ -11898,19 +12130,19 @@
       </c>
     </row>
     <row r="85" spans="1:12">
-      <c r="A85" s="126" t="s">
+      <c r="A85" s="125" t="s">
         <v>720</v>
       </c>
       <c r="B85" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="131" t="s">
+      <c r="C85" s="127" t="s">
         <v>942</v>
       </c>
       <c r="D85" s="108" t="s">
         <v>421</v>
       </c>
-      <c r="E85" s="132" t="s">
+      <c r="E85" s="128" t="s">
         <v>986</v>
       </c>
       <c r="F85" s="113" t="s">
@@ -11930,19 +12162,19 @@
       </c>
     </row>
     <row r="86" spans="1:12">
-      <c r="A86" s="126" t="s">
+      <c r="A86" s="125" t="s">
         <v>713</v>
       </c>
       <c r="B86" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C86" s="131" t="s">
+      <c r="C86" s="127" t="s">
         <v>943</v>
       </c>
       <c r="D86" s="108" t="s">
         <v>414</v>
       </c>
-      <c r="E86" s="132" t="s">
+      <c r="E86" s="128" t="s">
         <v>990</v>
       </c>
       <c r="F86" s="113" t="s">
@@ -11962,19 +12194,19 @@
       </c>
     </row>
     <row r="87" spans="1:12">
-      <c r="A87" s="126" t="s">
+      <c r="A87" s="125" t="s">
         <v>741</v>
       </c>
       <c r="B87" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C87" s="131" t="s">
+      <c r="C87" s="127" t="s">
         <v>944</v>
       </c>
       <c r="D87" s="108" t="s">
         <v>429</v>
       </c>
-      <c r="E87" s="132" t="s">
+      <c r="E87" s="128" t="s">
         <v>995</v>
       </c>
       <c r="F87" s="113" t="s">
@@ -11994,19 +12226,19 @@
       </c>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="126" t="s">
+      <c r="A88" s="125" t="s">
         <v>931</v>
       </c>
       <c r="B88" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C88" s="131" t="s">
+      <c r="C88" s="127" t="s">
         <v>945</v>
       </c>
       <c r="D88" s="108" t="s">
         <v>994</v>
       </c>
-      <c r="E88" s="132" t="s">
+      <c r="E88" s="128" t="s">
         <v>996</v>
       </c>
       <c r="F88" s="113" t="s">
@@ -12026,19 +12258,19 @@
       </c>
     </row>
     <row r="89" spans="1:12">
-      <c r="A89" s="126" t="s">
+      <c r="A89" s="125" t="s">
         <v>932</v>
       </c>
       <c r="B89" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C89" s="131" t="s">
+      <c r="C89" s="127" t="s">
         <v>946</v>
       </c>
       <c r="D89" s="108" t="s">
         <v>702</v>
       </c>
-      <c r="E89" s="132" t="s">
+      <c r="E89" s="128" t="s">
         <v>999</v>
       </c>
       <c r="F89" s="113" t="s">
@@ -12058,19 +12290,19 @@
       </c>
     </row>
     <row r="90" spans="1:12">
-      <c r="A90" s="126" t="s">
+      <c r="A90" s="125" t="s">
         <v>933</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C90" s="131" t="s">
+      <c r="C90" s="127" t="s">
         <v>947</v>
       </c>
       <c r="D90" s="108" t="s">
         <v>444</v>
       </c>
-      <c r="E90" s="132" t="s">
+      <c r="E90" s="128" t="s">
         <v>1008</v>
       </c>
       <c r="F90" s="113" t="s">
@@ -12090,19 +12322,19 @@
       </c>
     </row>
     <row r="91" spans="1:12">
-      <c r="A91" s="126" t="s">
+      <c r="A91" s="125" t="s">
         <v>934</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="131" t="s">
+      <c r="C91" s="127" t="s">
         <v>948</v>
       </c>
       <c r="D91" s="108" t="s">
         <v>1007</v>
       </c>
-      <c r="E91" s="132" t="s">
+      <c r="E91" s="128" t="s">
         <v>1009</v>
       </c>
       <c r="F91" s="113" t="s">
@@ -12122,16 +12354,16 @@
       </c>
     </row>
     <row r="92" spans="1:12">
-      <c r="A92" s="126" t="s">
+      <c r="A92" s="125" t="s">
         <v>935</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D92" s="109" t="s">
         <v>848</v>
       </c>
-      <c r="E92" s="132" t="s">
+      <c r="E92" s="128" t="s">
         <v>255</v>
       </c>
       <c r="F92" s="113" t="s">
@@ -12151,7 +12383,7 @@
       </c>
     </row>
     <row r="93" spans="1:12">
-      <c r="A93" s="126" t="s">
+      <c r="A93" s="125" t="s">
         <v>936</v>
       </c>
       <c r="B93" s="10" t="s">
@@ -12160,10 +12392,10 @@
       <c r="C93" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="D93" s="108" t="s">
+      <c r="D93" s="109" t="s">
         <v>708</v>
       </c>
-      <c r="E93" s="132" t="s">
+      <c r="E93" s="128" t="s">
         <v>76</v>
       </c>
       <c r="F93" s="113" t="s">
@@ -12186,7 +12418,7 @@
       </c>
     </row>
     <row r="94" spans="1:12">
-      <c r="A94" s="126" t="s">
+      <c r="A94" s="125" t="s">
         <v>937</v>
       </c>
       <c r="B94" s="10" t="s">
@@ -12198,7 +12430,7 @@
       <c r="D94" s="108" t="s">
         <v>344</v>
       </c>
-      <c r="E94" s="132" t="s">
+      <c r="E94" s="128" t="s">
         <v>223</v>
       </c>
       <c r="F94" s="113" t="s">
@@ -12221,7 +12453,7 @@
       </c>
     </row>
     <row r="95" spans="1:12">
-      <c r="A95" s="126" t="s">
+      <c r="A95" s="125" t="s">
         <v>938</v>
       </c>
       <c r="B95" s="10" t="s">
@@ -12233,7 +12465,7 @@
       <c r="D95" s="108" t="s">
         <v>1014</v>
       </c>
-      <c r="E95" s="132" t="s">
+      <c r="E95" s="128" t="s">
         <v>261</v>
       </c>
       <c r="F95" s="113" t="s">
@@ -12253,13 +12485,13 @@
       </c>
     </row>
     <row r="96" spans="1:12">
-      <c r="A96" s="126" t="s">
+      <c r="A96" s="125" t="s">
         <v>912</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C96" s="131" t="s">
+      <c r="C96" s="127" t="s">
         <v>909</v>
       </c>
       <c r="D96" s="108" t="s">
@@ -12285,7 +12517,7 @@
       </c>
     </row>
     <row r="97" spans="1:12">
-      <c r="A97" s="126" t="s">
+      <c r="A97" s="125" t="s">
         <v>1046</v>
       </c>
       <c r="B97" s="10" t="s">
@@ -12323,7 +12555,7 @@
       </c>
     </row>
     <row r="98" spans="1:12">
-      <c r="A98" s="127" t="s">
+      <c r="A98" s="126" t="s">
         <v>1044</v>
       </c>
       <c r="B98" s="10" t="s">
@@ -12341,7 +12573,7 @@
       <c r="F98" s="10" t="s">
         <v>1017</v>
       </c>
-      <c r="G98" s="132" t="s">
+      <c r="G98" s="128" t="s">
         <v>255</v>
       </c>
       <c r="H98" s="111" t="s">
@@ -12361,7 +12593,7 @@
       </c>
     </row>
     <row r="99" spans="1:12">
-      <c r="A99" s="127" t="s">
+      <c r="A99" s="126" t="s">
         <v>1044</v>
       </c>
       <c r="B99" s="10" t="s">
@@ -12379,7 +12611,7 @@
       <c r="F99" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G99" s="132" t="s">
+      <c r="G99" s="128" t="s">
         <v>261</v>
       </c>
       <c r="H99" s="111" t="s">
@@ -12399,7 +12631,7 @@
       </c>
     </row>
     <row r="100" spans="1:12">
-      <c r="A100" s="127" t="s">
+      <c r="A100" s="126" t="s">
         <v>1044</v>
       </c>
       <c r="B100" s="10" t="s">
@@ -12417,7 +12649,7 @@
       <c r="F100" s="113" t="s">
         <v>389</v>
       </c>
-      <c r="G100" s="132" t="s">
+      <c r="G100" s="128" t="s">
         <v>1038</v>
       </c>
       <c r="H100" s="111" t="s">
@@ -12437,7 +12669,7 @@
       </c>
     </row>
     <row r="101" spans="1:12">
-      <c r="A101" s="127" t="s">
+      <c r="A101" s="126" t="s">
         <v>1044</v>
       </c>
       <c r="B101" s="10" t="s">
@@ -12455,7 +12687,7 @@
       <c r="F101" s="113" t="s">
         <v>380</v>
       </c>
-      <c r="G101" s="132" t="s">
+      <c r="G101" s="128" t="s">
         <v>1030</v>
       </c>
       <c r="H101" s="111" t="s">
@@ -12475,7 +12707,7 @@
       </c>
     </row>
     <row r="102" spans="1:12">
-      <c r="A102" s="127" t="s">
+      <c r="A102" s="126" t="s">
         <v>1044</v>
       </c>
       <c r="B102" s="10" t="s">
@@ -12493,7 +12725,7 @@
       <c r="F102" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="G102" s="132" t="s">
+      <c r="G102" s="128" t="s">
         <v>535</v>
       </c>
       <c r="H102" s="111" t="s">
@@ -12521,4 +12753,1970 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7498E122-41A9-4336-B180-463F02F789BB}">
+  <dimension ref="A1:AI38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="10" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="10" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" s="133" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="140" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="X1" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF1" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH1" s="55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" s="134"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="134"/>
+      <c r="V2" s="134"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="29"/>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3" s="134"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="29"/>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" s="134"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="134"/>
+      <c r="V4" s="134"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="28"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="28"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AI4" s="29"/>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" s="134"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="134"/>
+      <c r="V5" s="134"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AD5" s="28"/>
+      <c r="AE5" s="28"/>
+      <c r="AF5" s="28"/>
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="28"/>
+      <c r="AI5" s="29"/>
+    </row>
+    <row r="6" spans="1:35" ht="21" customHeight="1">
+      <c r="A6" s="134"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="134" t="s">
+        <v>1047</v>
+      </c>
+      <c r="V6" s="36">
+        <v>10</v>
+      </c>
+      <c r="W6" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="X6" s="52">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Y6" s="52"/>
+      <c r="Z6" s="53"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC6" s="51"/>
+      <c r="AD6" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="AE6" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF6" s="56">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="AG6" s="52"/>
+      <c r="AH6" s="52" t="s">
+        <v>314</v>
+      </c>
+      <c r="AI6" s="29"/>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" s="134"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="134" t="s">
+        <v>1047</v>
+      </c>
+      <c r="V7" s="43">
+        <v>12</v>
+      </c>
+      <c r="W7" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7" s="34">
+        <v>2.1</v>
+      </c>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB7" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE7" s="34"/>
+      <c r="AF7" s="42">
+        <v>8.4027777777777771E-2</v>
+      </c>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="AI7" s="29"/>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" s="134"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="134" t="s">
+        <v>1047</v>
+      </c>
+      <c r="V8" s="138">
+        <v>11</v>
+      </c>
+      <c r="W8" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="X8" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="52"/>
+      <c r="AA8" s="52" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB8" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC8" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD8" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE8" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF8" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG8" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH8" s="52" t="s">
+        <v>315</v>
+      </c>
+      <c r="AI8" s="29"/>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" s="134"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="V9" s="43">
+        <v>13</v>
+      </c>
+      <c r="W9" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="X9" s="34">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB9" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC9" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="34"/>
+      <c r="AF9" s="42">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="AI9" s="29"/>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" s="134"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="V10" s="36">
+        <v>40</v>
+      </c>
+      <c r="W10" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="X10" s="40">
+        <v>8.6111111111111124E-2</v>
+      </c>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="40">
+        <v>8.6111111111111124E-2</v>
+      </c>
+      <c r="AG10" s="31"/>
+      <c r="AH10" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI10" s="29"/>
+    </row>
+    <row r="11" spans="1:35" ht="22.5" customHeight="1">
+      <c r="A11" s="134"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="V11" s="43">
+        <v>41</v>
+      </c>
+      <c r="W11" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="X11" s="42">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA11" s="34"/>
+      <c r="AB11" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC11" s="34"/>
+      <c r="AD11" s="34"/>
+      <c r="AE11" s="34"/>
+      <c r="AF11" s="42">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="AG11" s="34"/>
+      <c r="AH11" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="AI11" s="29"/>
+    </row>
+    <row r="12" spans="1:35" ht="18.75" customHeight="1">
+      <c r="A12" s="134"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="V12" s="36">
+        <v>42</v>
+      </c>
+      <c r="W12" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="X12" s="40">
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="40">
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="AG12" s="31"/>
+      <c r="AH12" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI12" s="29"/>
+    </row>
+    <row r="13" spans="1:35">
+      <c r="A13" s="134"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="V13" s="43">
+        <v>43</v>
+      </c>
+      <c r="W13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="X13" s="42">
+        <v>8.819444444444445E-2</v>
+      </c>
+      <c r="Y13" s="34"/>
+      <c r="Z13" s="34"/>
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC13" s="34"/>
+      <c r="AD13" s="34"/>
+      <c r="AE13" s="34"/>
+      <c r="AF13" s="42">
+        <v>8.819444444444445E-2</v>
+      </c>
+      <c r="AG13" s="34"/>
+      <c r="AH13" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI13" s="29"/>
+    </row>
+    <row r="14" spans="1:35" ht="18.75" customHeight="1">
+      <c r="A14" s="134"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="V14" s="36">
+        <v>44</v>
+      </c>
+      <c r="W14" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="X14" s="40">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="40">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI14" s="29"/>
+    </row>
+    <row r="15" spans="1:35">
+      <c r="A15" s="134"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="134" t="s">
+        <v>190</v>
+      </c>
+      <c r="V15" s="43">
+        <v>45</v>
+      </c>
+      <c r="W15" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="X15" s="42">
+        <v>8.9583333333333334E-2</v>
+      </c>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="34"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="34"/>
+      <c r="AE15" s="34"/>
+      <c r="AF15" s="42">
+        <v>8.9583333333333334E-2</v>
+      </c>
+      <c r="AG15" s="34"/>
+      <c r="AH15" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI15" s="29"/>
+    </row>
+    <row r="16" spans="1:35">
+      <c r="A16" s="135">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="31"/>
+      <c r="L16" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" s="134" t="s">
+        <v>95</v>
+      </c>
+      <c r="V16" s="36">
+        <v>6</v>
+      </c>
+      <c r="W16" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="X16" s="31">
+        <v>2.1</v>
+      </c>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="40">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="AG16" s="51"/>
+      <c r="AH16" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="AI16" s="29"/>
+    </row>
+    <row r="17" spans="1:35">
+      <c r="A17" s="136">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" s="34"/>
+      <c r="L17" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="M17" s="134" t="s">
+        <v>101</v>
+      </c>
+      <c r="V17" s="43">
+        <v>9</v>
+      </c>
+      <c r="W17" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="X17" s="34">
+        <v>2.11</v>
+      </c>
+      <c r="Y17" s="34"/>
+      <c r="Z17" s="34"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC17" s="34"/>
+      <c r="AD17" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE17" s="34"/>
+      <c r="AF17" s="42">
+        <v>9.0972222222222218E-2</v>
+      </c>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="AI17" s="29"/>
+    </row>
+    <row r="18" spans="1:35">
+      <c r="A18" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="K18" s="101" t="s">
+        <v>217</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" s="134" t="s">
+        <v>175</v>
+      </c>
+      <c r="V18" s="36">
+        <v>32</v>
+      </c>
+      <c r="W18" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="X18" s="31">
+        <v>2.12</v>
+      </c>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE18" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF18" s="40">
+        <v>9.1666666666666674E-2</v>
+      </c>
+      <c r="AG18" s="51"/>
+      <c r="AH18" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="AI18" s="29"/>
+    </row>
+    <row r="19" spans="1:35">
+      <c r="A19" s="134">
+        <v>1.19</v>
+      </c>
+      <c r="B19" s="132" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="132" t="str">
+        <f>$I$18</f>
+        <v>3:11</v>
+      </c>
+      <c r="J19" s="132" t="s">
+        <v>1058</v>
+      </c>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="M19" s="144" t="s">
+        <v>1057</v>
+      </c>
+      <c r="V19" s="141">
+        <v>47</v>
+      </c>
+      <c r="W19" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="X19" s="29">
+        <v>2.13</v>
+      </c>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="29"/>
+      <c r="AC19" s="29"/>
+      <c r="AD19" s="29"/>
+      <c r="AE19" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="AF19" s="100">
+        <v>9.2361111111111116E-2</v>
+      </c>
+      <c r="AG19" s="29"/>
+      <c r="AH19" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="AI19" s="29"/>
+    </row>
+    <row r="20" spans="1:35" ht="24.75" customHeight="1">
+      <c r="A20" s="135">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="40">
+        <v>0.125</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="31"/>
+      <c r="L20" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="M20" s="134" t="s">
+        <v>83</v>
+      </c>
+      <c r="V20" s="142">
+        <v>48</v>
+      </c>
+      <c r="W20" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="X20" s="51">
+        <v>2.14</v>
+      </c>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51" t="s">
+        <v>272</v>
+      </c>
+      <c r="AF20" s="99">
+        <v>9.3055555555555558E-2</v>
+      </c>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="51" t="s">
+        <v>273</v>
+      </c>
+      <c r="AI20" s="29"/>
+    </row>
+    <row r="21" spans="1:35" ht="18.75" customHeight="1">
+      <c r="A21" s="134"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="134" t="s">
+        <v>192</v>
+      </c>
+      <c r="V21" s="141">
+        <v>49</v>
+      </c>
+      <c r="W21" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="X21" s="100">
+        <v>9.375E-2</v>
+      </c>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
+      <c r="AE21" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF21" s="100">
+        <v>9.375E-2</v>
+      </c>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="AI21" s="29"/>
+    </row>
+    <row r="22" spans="1:35">
+      <c r="A22" s="135">
+        <v>1.18</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="40">
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="31"/>
+      <c r="L22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="M22" s="134" t="s">
+        <v>64</v>
+      </c>
+      <c r="V22" s="36">
+        <v>8</v>
+      </c>
+      <c r="W22" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="X22" s="31">
+        <v>2.16</v>
+      </c>
+      <c r="Y22" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE22" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF22" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG22" s="51"/>
+      <c r="AH22" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="AI22" s="29"/>
+    </row>
+    <row r="23" spans="1:35">
+      <c r="A23" s="134" t="s">
+        <v>252</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="139">
+        <v>0.12777777777777777</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>1062</v>
+      </c>
+      <c r="K23" s="104" t="s">
+        <v>255</v>
+      </c>
+      <c r="L23" s="28" t="s">
+        <v>1052</v>
+      </c>
+      <c r="M23" s="144">
+        <v>64</v>
+      </c>
+      <c r="V23" s="43">
+        <v>7</v>
+      </c>
+      <c r="W23" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="X23" s="34">
+        <v>2.17</v>
+      </c>
+      <c r="Y23" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE23" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF23" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="AI23" s="29"/>
+    </row>
+    <row r="24" spans="1:35" ht="16.5" customHeight="1">
+      <c r="A24" s="136">
+        <v>1.17</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="42">
+        <v>0.12569444444444444</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="K24" s="29"/>
+      <c r="L24" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="134" t="s">
+        <v>77</v>
+      </c>
+      <c r="V24" s="36" t="s">
+        <v>1049</v>
+      </c>
+      <c r="W24" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="X24" s="31">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
+      <c r="AA24" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB24" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE24" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF24" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG24" s="51"/>
+      <c r="AH24" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="AI24" s="29"/>
+    </row>
+    <row r="25" spans="1:35" ht="17.25" customHeight="1">
+      <c r="A25" s="136">
+        <v>1.24</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" s="34"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42">
+        <v>0.13055555555555556</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="K25" s="102" t="s">
+        <v>218</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="M25" s="134" t="s">
+        <v>150</v>
+      </c>
+      <c r="V25" s="43" t="s">
+        <v>1048</v>
+      </c>
+      <c r="W25" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="X25" s="34">
+        <v>2.19</v>
+      </c>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB25" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE25" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF25" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG25" s="29"/>
+      <c r="AH25" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="AI25" s="29"/>
+    </row>
+    <row r="26" spans="1:35" ht="16.5" customHeight="1">
+      <c r="A26" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="G26" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="H26" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="J26" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="K26" s="103" t="s">
+        <v>214</v>
+      </c>
+      <c r="L26" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="M26" s="134" t="s">
+        <v>182</v>
+      </c>
+      <c r="V26" s="142">
+        <v>52</v>
+      </c>
+      <c r="W26" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="X26" s="99">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="Y26" s="51"/>
+      <c r="Z26" s="57"/>
+      <c r="AA26" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="AB26" s="51"/>
+      <c r="AC26" s="51"/>
+      <c r="AD26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51" t="s">
+        <v>279</v>
+      </c>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="51" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI26" s="29"/>
+    </row>
+    <row r="27" spans="1:35" ht="18.75" customHeight="1">
+      <c r="A27" s="135">
+        <v>1.25</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="31"/>
+      <c r="I27" s="40">
+        <v>0.13125000000000001</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="K27" s="104" t="s">
+        <v>94</v>
+      </c>
+      <c r="L27" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="M27" s="134" t="s">
+        <v>89</v>
+      </c>
+      <c r="V27" s="141">
+        <v>53</v>
+      </c>
+      <c r="W27" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="X27" s="100">
+        <v>9.7916666666666666E-2</v>
+      </c>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="AI27" s="29"/>
+    </row>
+    <row r="28" spans="1:35">
+      <c r="A28" s="134" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="139">
+        <v>0.12847222222222221</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>1063</v>
+      </c>
+      <c r="K28" s="104" t="s">
+        <v>261</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="M28" s="144">
+        <v>65</v>
+      </c>
+      <c r="V28" s="141">
+        <v>54</v>
+      </c>
+      <c r="W28" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="X28" s="99">
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="Y28" s="51"/>
+      <c r="Z28" s="57"/>
+      <c r="AA28" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB28" s="51"/>
+      <c r="AC28" s="51"/>
+      <c r="AD28" s="51"/>
+      <c r="AE28" s="51"/>
+      <c r="AF28" s="51" t="s">
+        <v>284</v>
+      </c>
+      <c r="AG28" s="51"/>
+      <c r="AH28" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI28" s="29"/>
+    </row>
+    <row r="29" spans="1:35" ht="17.25" customHeight="1">
+      <c r="A29" s="134" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="139">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J29" s="139">
+        <v>8.4027777777777785E-2</v>
+      </c>
+      <c r="K29" s="104" t="s">
+        <v>219</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>1054</v>
+      </c>
+      <c r="M29" s="144">
+        <v>66</v>
+      </c>
+      <c r="V29" s="141">
+        <v>55</v>
+      </c>
+      <c r="W29" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="X29" s="100">
+        <v>9.930555555555555E-2</v>
+      </c>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="60"/>
+      <c r="AA29" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB29" s="29"/>
+      <c r="AC29" s="29"/>
+      <c r="AD29" s="29"/>
+      <c r="AE29" s="29"/>
+      <c r="AF29" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="AG29" s="29"/>
+      <c r="AH29" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="AI29" s="29"/>
+    </row>
+    <row r="30" spans="1:35">
+      <c r="A30" s="134" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="139">
+        <v>0.13402777777777777</v>
+      </c>
+      <c r="J30" s="139">
+        <v>8.4722222222222227E-2</v>
+      </c>
+      <c r="K30" s="104" t="s">
+        <v>220</v>
+      </c>
+      <c r="L30" s="28" t="s">
+        <v>1055</v>
+      </c>
+      <c r="M30" s="144">
+        <v>67</v>
+      </c>
+      <c r="V30" s="141">
+        <v>56</v>
+      </c>
+      <c r="W30" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="X30" s="99">
+        <v>0.1</v>
+      </c>
+      <c r="Y30" s="51"/>
+      <c r="Z30" s="57"/>
+      <c r="AA30" s="51"/>
+      <c r="AB30" s="51" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51" t="s">
+        <v>288</v>
+      </c>
+      <c r="AG30" s="51"/>
+      <c r="AH30" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="AI30" s="29"/>
+    </row>
+    <row r="31" spans="1:35" ht="18.75" customHeight="1">
+      <c r="A31" s="134" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="139">
+        <v>0.13472222222222222</v>
+      </c>
+      <c r="J31" s="139">
+        <v>8.5416666666666669E-2</v>
+      </c>
+      <c r="K31" s="104" t="s">
+        <v>236</v>
+      </c>
+      <c r="L31" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="M31" s="144">
+        <v>26</v>
+      </c>
+      <c r="V31" s="141">
+        <v>57</v>
+      </c>
+      <c r="W31" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="X31" s="100">
+        <v>0.10069444444444445</v>
+      </c>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="60"/>
+      <c r="AA31" s="29"/>
+      <c r="AB31" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="AC31" s="29"/>
+      <c r="AD31" s="29"/>
+      <c r="AE31" s="29"/>
+      <c r="AF31" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="AG31" s="29"/>
+      <c r="AH31" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="AI31" s="29"/>
+    </row>
+    <row r="32" spans="1:35">
+      <c r="A32" s="137">
+        <v>1.2</v>
+      </c>
+      <c r="B32" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="49"/>
+      <c r="D32" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="M32" s="134">
+        <v>1</v>
+      </c>
+      <c r="V32" s="141">
+        <v>58</v>
+      </c>
+      <c r="W32" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="X32" s="100">
+        <v>0.10138888888888889</v>
+      </c>
+      <c r="Y32" s="51"/>
+      <c r="Z32" s="57"/>
+      <c r="AA32" s="51"/>
+      <c r="AB32" s="51" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC32" s="51"/>
+      <c r="AD32" s="51"/>
+      <c r="AE32" s="51"/>
+      <c r="AF32" s="51" t="s">
+        <v>294</v>
+      </c>
+      <c r="AG32" s="29"/>
+      <c r="AH32" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="AI32" s="29"/>
+    </row>
+    <row r="33" spans="1:35" ht="17.25" customHeight="1">
+      <c r="A33" s="138">
+        <v>1.3</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="53"/>
+      <c r="D33" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="M33" s="134">
+        <v>0</v>
+      </c>
+      <c r="V33" s="141">
+        <v>59</v>
+      </c>
+      <c r="W33" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="X33" s="100">
+        <v>0.10208333333333333</v>
+      </c>
+      <c r="Y33" s="29"/>
+      <c r="Z33" s="60"/>
+      <c r="AA33" s="29"/>
+      <c r="AB33" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC33" s="29"/>
+      <c r="AD33" s="29"/>
+      <c r="AE33" s="29"/>
+      <c r="AF33" s="29"/>
+      <c r="AG33" s="29"/>
+      <c r="AH33" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="AI33" s="29"/>
+    </row>
+    <row r="34" spans="1:35" ht="18" customHeight="1">
+      <c r="A34" s="136" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="I34" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" s="105" t="s">
+        <v>216</v>
+      </c>
+      <c r="L34" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M34" s="134" t="s">
+        <v>70</v>
+      </c>
+      <c r="V34" s="36" t="s">
+        <v>1050</v>
+      </c>
+      <c r="W34" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="X34" s="31">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="Y34" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z34" s="31"/>
+      <c r="AA34" s="31"/>
+      <c r="AB34" s="31"/>
+      <c r="AC34" s="31"/>
+      <c r="AD34" s="31"/>
+      <c r="AE34" s="31"/>
+      <c r="AF34" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG34" s="29"/>
+      <c r="AH34" s="102" t="s">
+        <v>255</v>
+      </c>
+      <c r="AI34" s="29"/>
+    </row>
+    <row r="35" spans="1:35" ht="17.25" customHeight="1">
+      <c r="A35" s="135" t="s">
+        <v>205</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="I35" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="J35" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="K35" s="104" t="s">
+        <v>215</v>
+      </c>
+      <c r="L35" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="M35" s="134" t="s">
+        <v>157</v>
+      </c>
+      <c r="V35" s="43" t="s">
+        <v>1051</v>
+      </c>
+      <c r="W35" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="X35" s="34">
+        <v>2.29</v>
+      </c>
+      <c r="Y35" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z35" s="34"/>
+      <c r="AA35" s="34"/>
+      <c r="AB35" s="34"/>
+      <c r="AC35" s="34"/>
+      <c r="AD35" s="34"/>
+      <c r="AE35" s="34"/>
+      <c r="AF35" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG35" s="29"/>
+      <c r="AH35" s="102" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI35" s="29"/>
+    </row>
+    <row r="36" spans="1:35" ht="15.75" customHeight="1">
+      <c r="A36" s="136">
+        <v>1.31</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H36" s="34"/>
+      <c r="I36" s="42">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="J36" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="K36" s="106" t="s">
+        <v>113</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="M36" s="134" t="s">
+        <v>108</v>
+      </c>
+      <c r="V36" s="141">
+        <v>62</v>
+      </c>
+      <c r="W36" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="X36" s="100">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="Y36" s="29"/>
+      <c r="Z36" s="29"/>
+      <c r="AA36" s="29"/>
+      <c r="AB36" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="AC36" s="29"/>
+      <c r="AD36" s="29"/>
+      <c r="AE36" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="AF36" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG36" s="29"/>
+      <c r="AH36" s="102" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI36" s="29"/>
+    </row>
+    <row r="37" spans="1:35" ht="18" customHeight="1">
+      <c r="A37" s="134"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="134" t="s">
+        <v>191</v>
+      </c>
+      <c r="V37" s="141">
+        <v>63</v>
+      </c>
+      <c r="W37" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="X37" s="100">
+        <v>0.10486111111111111</v>
+      </c>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="AC37" s="29"/>
+      <c r="AD37" s="29"/>
+      <c r="AE37" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF37" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG37" s="29"/>
+      <c r="AH37" s="102" t="s">
+        <v>261</v>
+      </c>
+      <c r="AI37" s="29"/>
+    </row>
+    <row r="38" spans="1:35" ht="4.5" customHeight="1"/>
+  </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
+  <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
+  <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>